<commit_message>
Added page object model
</commit_message>
<xml_diff>
--- a/EmployeeManagement/Test Data/Orange_data.xlsx
+++ b/EmployeeManagement/Test Data/Orange_data.xlsx
@@ -5,16 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\snehaps\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AutomationTraining\AutomationFramework\EmployeeManagement\Test Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2112CDAD-9DE3-4A13-829A-F7B5DE84491F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E44CD429-B890-42FF-9C7B-A3F8C4163469}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="10200" xr2:uid="{4C92DB80-EE66-45D3-87CE-9F8A91CAD6FF}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{4C92DB80-EE66-45D3-87CE-9F8A91CAD6FF}"/>
   </bookViews>
   <sheets>
     <sheet name="InvalidLoginTest" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="AddValidEmployeeTest" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>username</t>
   </si>
@@ -48,9 +48,6 @@
     <t>Admin</t>
   </si>
   <si>
-    <t>admin123</t>
-  </si>
-  <si>
     <t>expectedError</t>
   </si>
   <si>
@@ -63,22 +60,22 @@
     <t>john123</t>
   </si>
   <si>
-    <t>peter</t>
-  </si>
-  <si>
-    <t>peter123</t>
-  </si>
-  <si>
-    <t>saul</t>
-  </si>
-  <si>
-    <t>saul123</t>
-  </si>
-  <si>
-    <t>jack</t>
-  </si>
-  <si>
-    <t>jack123</t>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>First Name</t>
+  </si>
+  <si>
+    <t>Middle Name</t>
+  </si>
+  <si>
+    <t>Last Name</t>
+  </si>
+  <si>
+    <t>Expected Employee Name</t>
   </si>
 </sst>
 </file>
@@ -110,7 +107,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -133,14 +130,29 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -455,119 +467,109 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C317292E-B3BC-45A4-9E74-4B3253B0349C}">
-  <dimension ref="B2:D14"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="9.54296875" customWidth="1"/>
-    <col min="3" max="3" width="10" customWidth="1"/>
+    <col min="3" max="3" width="15.1796875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B2" s="1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" s="2" t="s">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B6" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B7" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-    </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-    </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-    </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-    </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-    </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-    </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
+      <c r="B3" s="2">
+        <v>123</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="3"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -577,12 +579,41 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2B114BB-498C-4446-94FD-01378496E932}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J17" activeCellId="1" sqref="F6 J17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <cols>
+    <col min="3" max="3" width="10.7265625" customWidth="1"/>
+    <col min="4" max="4" width="12" customWidth="1"/>
+    <col min="5" max="5" width="10.453125" customWidth="1"/>
+    <col min="6" max="6" width="23.26953125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>